<commit_message>
Reorganized files, added stats results
</commit_message>
<xml_diff>
--- a/lit-review/dl4se.xlsx
+++ b/lit-review/dl4se.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hyp" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,72 +437,77 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Convolutional</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DNN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Feedforward</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Sequence</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Convolutional</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Attention</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Embedding</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Feedforward</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>DNN</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>word2vec</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Graph</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>word2vec</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Attention</t>
-        </is>
-      </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Deep Belief Network</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Code Synthesis</t>
+          <t>Clone Detection</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -521,34 +526,37 @@
       </c>
       <c r="K2" t="n">
         <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>code comprehension</t>
+          <t>Code Synthesis</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -558,16 +566,19 @@
       </c>
       <c r="K3" t="n">
         <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>language model</t>
+          <t>Feature Envy Detection</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -595,25 +606,28 @@
       </c>
       <c r="K4" t="n">
         <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>language processing</t>
+          <t>Program Repair</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -622,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -632,59 +646,65 @@
       </c>
       <c r="K5" t="n">
         <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>defect prediction</t>
+          <t>Software Categorization</t>
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
         <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Clone Detection</t>
+          <t>Software Energy Metrics</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -693,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -706,16 +726,19 @@
       </c>
       <c r="K7" t="n">
         <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Program Repair</t>
+          <t>Testing</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -727,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -736,13 +759,16 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -752,16 +778,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -776,20 +802,23 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Software Categorization</t>
+          <t>bug localization</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -807,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -817,16 +846,19 @@
       </c>
       <c r="K10" t="n">
         <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>bug localization</t>
+          <t>code comprehension</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -835,38 +867,41 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Feature Envy Detection</t>
+          <t>code smell</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -878,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -891,16 +926,19 @@
       </c>
       <c r="K12" t="n">
         <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Software Energy Metrics</t>
+          <t>defect prediction</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -909,13 +947,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -927,17 +965,20 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>code smell</t>
+          <t>image processing</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -965,25 +1006,28 @@
       </c>
       <c r="K14" t="n">
         <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>image processing</t>
+          <t>issue close time</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1002,6 +1046,129 @@
       </c>
       <c r="K15" t="n">
         <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>language model</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>9</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>language processing</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>18</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>58</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3</v>
+      </c>
+      <c r="I18" t="n">
+        <v>4</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>